<commit_message>
Add minor changes to CRUD matrix
</commit_message>
<xml_diff>
--- a/CRUD.xlsx
+++ b/CRUD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Studia\Semestr 5\BD2\Projekt\Macierz CRUD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Studia\Semestr 5\BD2\Projekt\BD2_20Z_Rekrutacja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B190E8-FAF7-4500-909D-30FDAF44C0C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420C71DE-00DD-4414-8597-8D2ADA933D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A8FA609-6934-4543-8C90-936948A4517A}"/>
   </bookViews>
@@ -991,82 +991,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFEAF01-52CE-4CCD-9AD6-DCF462E5F2A8}">
   <dimension ref="A1:AB216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="18" width="7.140625" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="35"/>
+    <col min="2" max="2" width="6.7109375" style="35" customWidth="1"/>
+    <col min="3" max="21" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="214.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>48</v>
+      <c r="U1" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
@@ -1076,36 +1074,36 @@
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="B2" s="21"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="D2" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="I2" s="14"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="L2" s="14"/>
       <c r="M2" s="9"/>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="14" t="s">
         <v>37</v>
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
-      <c r="R2" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="21"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1115,33 +1113,33 @@
       <c r="A3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+      <c r="L3" s="15"/>
       <c r="M3" s="10"/>
-      <c r="N3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="N3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
-      <c r="R3" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="10"/>
-      <c r="T3" s="15"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="10"/>
       <c r="U3" s="10"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
@@ -1155,41 +1153,41 @@
       <c r="B4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="I4" s="16"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="L4" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="16"/>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="16"/>
+      <c r="Q4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="S4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="T4" s="16"/>
-      <c r="U4" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="T4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" s="11"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -1200,58 +1198,58 @@
         <v>32</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>40</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F5" s="10" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="15" t="s">
         <v>40</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>37</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>37</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5" s="15"/>
       <c r="O5" s="10" t="s">
         <v>40</v>
       </c>
       <c r="P5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1269,18 +1267,18 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="I6" s="16"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="N6" s="16"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
-      <c r="R6" s="16"/>
+      <c r="R6" s="11"/>
       <c r="S6" s="11"/>
-      <c r="T6" s="16"/>
+      <c r="T6" s="11"/>
       <c r="U6" s="11"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1291,37 +1289,37 @@
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="B7" s="10"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="R7" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="S7" s="10"/>
-      <c r="T7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="10"/>
       <c r="U7" s="10"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1332,41 +1330,41 @@
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="s">
         <v>37</v>
       </c>
       <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="K8" s="11"/>
-      <c r="L8" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="L8" s="16"/>
+      <c r="M8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
       <c r="Q8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="R8" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="S8" s="11"/>
-      <c r="T8" s="16"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="11"/>
       <c r="U8" s="11"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
@@ -1384,18 +1382,18 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="L9" s="15"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
+      <c r="N9" s="15"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
-      <c r="R9" s="15"/>
+      <c r="R9" s="10"/>
       <c r="S9" s="10"/>
-      <c r="T9" s="15"/>
+      <c r="T9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
@@ -1409,41 +1407,41 @@
       <c r="B10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11" t="s">
         <v>37</v>
       </c>
       <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="O10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="P10" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="16"/>
+      <c r="M10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="16"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
       <c r="Q10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="R10" s="16"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
@@ -1456,32 +1454,32 @@
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="G11" s="10"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="10"/>
+      <c r="N11" s="15"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T11" s="15"/>
+      <c r="Q11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="U11" s="10"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -1495,40 +1493,40 @@
       <c r="B12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>42</v>
-      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="H12" s="11"/>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="16"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="L12" s="16"/>
       <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
+      <c r="N12" s="16"/>
       <c r="O12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="16"/>
+      <c r="P12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R12" s="11"/>
       <c r="S12" s="11"/>
-      <c r="T12" s="16"/>
+      <c r="T12" s="11"/>
       <c r="U12" s="11" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
@@ -1539,19 +1537,19 @@
       <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="15"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1559,7 +1557,7 @@
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="15"/>
+      <c r="T13" s="10"/>
       <c r="U13" s="10"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
@@ -1573,31 +1571,31 @@
       <c r="B14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="L14" s="16"/>
       <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
-      <c r="R14" s="16"/>
+      <c r="R14" s="11"/>
       <c r="S14" s="11"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -1610,28 +1608,28 @@
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="G15" s="10"/>
       <c r="H15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10" t="s">
+      <c r="I15" s="15"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
-      <c r="R15" s="15"/>
+      <c r="R15" s="10"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="15"/>
+      <c r="T15" s="10"/>
       <c r="U15" s="10"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -1649,18 +1647,18 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="I16" s="16"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
+      <c r="N16" s="16"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
-      <c r="R16" s="16"/>
+      <c r="R16" s="11"/>
       <c r="S16" s="11"/>
-      <c r="T16" s="16"/>
+      <c r="T16" s="11"/>
       <c r="U16" s="11"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
@@ -1674,32 +1672,32 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="F17" s="10"/>
-      <c r="G17" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" s="10"/>
+      <c r="N17" s="15"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T17" s="15"/>
+      <c r="Q17" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="R17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="U17" s="10"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -1713,32 +1711,32 @@
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="E18" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="F18" s="11"/>
-      <c r="G18" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="G18" s="11"/>
       <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="I18" s="16"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="L18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="N18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="11"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="T18" s="16"/>
+      <c r="Q18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="U18" s="11"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
@@ -1752,32 +1750,32 @@
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="G19" s="10"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="L19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19" s="10"/>
+      <c r="N19" s="15"/>
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T19" s="15"/>
+      <c r="Q19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="U19" s="10"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
@@ -1791,32 +1789,32 @@
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="E20" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="I20" s="16"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="N20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20" s="11"/>
+      <c r="N20" s="16"/>
       <c r="O20" s="11"/>
       <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="T20" s="16"/>
+      <c r="Q20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="U20" s="11"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
@@ -1830,24 +1828,24 @@
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F21" s="10"/>
-      <c r="G21" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
+      <c r="I21" s="15"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
+      <c r="L21" s="15"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
+      <c r="N21" s="15"/>
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
-      <c r="R21" s="15"/>
+      <c r="R21" s="10"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="15"/>
+      <c r="T21" s="10"/>
       <c r="U21" s="10"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
@@ -1863,28 +1861,28 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="G22" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="O22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="P22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="R22" s="16"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N22" s="16"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="T22" s="11"/>
       <c r="U22" s="11"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
@@ -1896,33 +1894,33 @@
         <v>26</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
+      <c r="L23" s="15"/>
       <c r="M23" s="10"/>
-      <c r="N23" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="N23" s="15"/>
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
@@ -1932,30 +1930,30 @@
       <c r="A24" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="21"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="22"/>
       <c r="I24" s="21"/>
       <c r="J24" s="21"/>
-      <c r="K24" s="23" t="s">
+      <c r="K24" s="21"/>
+      <c r="L24" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="L24" s="21"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
-      <c r="O24" s="24"/>
+      <c r="O24" s="21"/>
       <c r="P24" s="21"/>
-      <c r="Q24" s="24"/>
+      <c r="Q24" s="21"/>
       <c r="R24" s="21"/>
-      <c r="S24" s="24" t="s">
+      <c r="S24" s="21"/>
+      <c r="T24" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="T24" s="21"/>
-      <c r="U24" s="26"/>
+      <c r="U24" s="21"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
@@ -1965,30 +1963,30 @@
       <c r="A25" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="10"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="15"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
-      <c r="K25" s="27" t="s">
+      <c r="K25" s="10"/>
+      <c r="L25" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
-      <c r="O25" s="27"/>
+      <c r="O25" s="10"/>
       <c r="P25" s="10"/>
-      <c r="Q25" s="27"/>
+      <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
-      <c r="S25" s="27" t="s">
+      <c r="S25" s="10"/>
+      <c r="T25" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="T25" s="10"/>
-      <c r="U25" s="28"/>
+      <c r="U25" s="10"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -1998,26 +1996,26 @@
       <c r="A26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="11"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="G26" s="30"/>
       <c r="H26" s="16"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="30"/>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
-      <c r="O26" s="30"/>
+      <c r="O26" s="11"/>
       <c r="P26" s="11"/>
-      <c r="Q26" s="30"/>
+      <c r="Q26" s="11"/>
       <c r="R26" s="11"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="31"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="11"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
@@ -2027,28 +2025,28 @@
       <c r="A27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="10"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="15"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="27"/>
       <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="27"/>
+      <c r="N27" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="O27" s="10"/>
       <c r="P27" s="10"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="S27" s="27"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="28"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="10"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
@@ -2058,28 +2056,28 @@
       <c r="A28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="11"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="G28" s="30"/>
       <c r="H28" s="16"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="30"/>
       <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="30"/>
+      <c r="N28" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O28" s="11"/>
       <c r="P28" s="11"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="S28" s="30"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="31"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="11"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
@@ -2089,59 +2087,59 @@
       <c r="A29" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="10"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="15"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="27"/>
       <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="27"/>
+      <c r="N29" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O29" s="10"/>
       <c r="P29" s="10"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="S29" s="27"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="28"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="10"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
     </row>
-    <row r="30" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="13"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="G30" s="33"/>
       <c r="H30" s="17"/>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="33"/>
       <c r="M30" s="13"/>
-      <c r="N30" s="13" t="s">
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="O30" s="33"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="33"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="33"/>
-      <c r="T30" s="13"/>
-      <c r="U30" s="34"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="13"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
@@ -2149,7 +2147,7 @@
     </row>
     <row r="31" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
-      <c r="B31" s="1"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -2168,7 +2166,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
-      <c r="U31" s="20"/>
+      <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
@@ -2176,7 +2174,7 @@
     </row>
     <row r="32" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2195,7 +2193,7 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
-      <c r="U32" s="20"/>
+      <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
@@ -2203,7 +2201,7 @@
     </row>
     <row r="33" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -2222,7 +2220,7 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
-      <c r="U33" s="20"/>
+      <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
@@ -2230,7 +2228,7 @@
     </row>
     <row r="34" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2249,7 +2247,7 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
-      <c r="U34" s="20"/>
+      <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
@@ -2257,7 +2255,7 @@
     </row>
     <row r="35" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="B35" s="20"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -2276,7 +2274,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
-      <c r="U35" s="20"/>
+      <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
@@ -2284,7 +2282,7 @@
     </row>
     <row r="36" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+      <c r="B36" s="20"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -2303,7 +2301,7 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
-      <c r="U36" s="20"/>
+      <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
@@ -2311,7 +2309,7 @@
     </row>
     <row r="37" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -2330,7 +2328,7 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
-      <c r="U37" s="20"/>
+      <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
@@ -2338,7 +2336,7 @@
     </row>
     <row r="38" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2357,7 +2355,7 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
-      <c r="U38" s="20"/>
+      <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
@@ -2365,7 +2363,7 @@
     </row>
     <row r="39" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -2384,7 +2382,7 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
-      <c r="U39" s="20"/>
+      <c r="U39" s="1"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
@@ -2392,7 +2390,7 @@
     </row>
     <row r="40" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
+      <c r="B40" s="20"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2411,7 +2409,7 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
-      <c r="U40" s="20"/>
+      <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
@@ -2419,7 +2417,7 @@
     </row>
     <row r="41" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="B41" s="20"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2438,7 +2436,7 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
-      <c r="U41" s="20"/>
+      <c r="U41" s="1"/>
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
@@ -2446,7 +2444,7 @@
     </row>
     <row r="42" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -2465,7 +2463,7 @@
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
-      <c r="U42" s="20"/>
+      <c r="U42" s="1"/>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
@@ -2473,7 +2471,7 @@
     </row>
     <row r="43" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2492,7 +2490,7 @@
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
-      <c r="U43" s="20"/>
+      <c r="U43" s="1"/>
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
@@ -2500,7 +2498,7 @@
     </row>
     <row r="44" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2519,7 +2517,7 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
-      <c r="U44" s="20"/>
+      <c r="U44" s="1"/>
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
@@ -2527,7 +2525,7 @@
     </row>
     <row r="45" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
+      <c r="B45" s="20"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2546,7 +2544,7 @@
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
-      <c r="U45" s="20"/>
+      <c r="U45" s="1"/>
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
@@ -2554,7 +2552,7 @@
     </row>
     <row r="46" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
+      <c r="B46" s="20"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -2573,7 +2571,7 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
-      <c r="U46" s="20"/>
+      <c r="U46" s="1"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
@@ -2581,7 +2579,7 @@
     </row>
     <row r="47" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="B47" s="20"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -2600,7 +2598,7 @@
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
-      <c r="U47" s="20"/>
+      <c r="U47" s="1"/>
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
@@ -2608,7 +2606,7 @@
     </row>
     <row r="48" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
+      <c r="B48" s="20"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -2627,7 +2625,7 @@
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
-      <c r="U48" s="20"/>
+      <c r="U48" s="1"/>
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
@@ -2635,7 +2633,7 @@
     </row>
     <row r="49" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="B49" s="20"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -2654,7 +2652,7 @@
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
-      <c r="U49" s="20"/>
+      <c r="U49" s="1"/>
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
@@ -2662,7 +2660,7 @@
     </row>
     <row r="50" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
+      <c r="B50" s="20"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2681,7 +2679,7 @@
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
-      <c r="U50" s="20"/>
+      <c r="U50" s="1"/>
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
@@ -2689,7 +2687,7 @@
     </row>
     <row r="51" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
+      <c r="B51" s="20"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -2708,7 +2706,7 @@
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
-      <c r="U51" s="20"/>
+      <c r="U51" s="1"/>
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
@@ -2716,7 +2714,7 @@
     </row>
     <row r="52" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
+      <c r="B52" s="20"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -2735,7 +2733,7 @@
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
-      <c r="U52" s="20"/>
+      <c r="U52" s="1"/>
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
@@ -2743,7 +2741,7 @@
     </row>
     <row r="53" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
+      <c r="B53" s="20"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -2762,7 +2760,7 @@
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
-      <c r="U53" s="20"/>
+      <c r="U53" s="1"/>
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
@@ -2770,7 +2768,7 @@
     </row>
     <row r="54" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
+      <c r="B54" s="20"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -2789,7 +2787,7 @@
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
-      <c r="U54" s="20"/>
+      <c r="U54" s="1"/>
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
@@ -2797,7 +2795,7 @@
     </row>
     <row r="55" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
+      <c r="B55" s="20"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -2816,7 +2814,7 @@
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
-      <c r="U55" s="20"/>
+      <c r="U55" s="1"/>
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
@@ -2824,7 +2822,7 @@
     </row>
     <row r="56" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
+      <c r="B56" s="20"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2843,7 +2841,7 @@
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
-      <c r="U56" s="20"/>
+      <c r="U56" s="1"/>
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
@@ -2851,7 +2849,7 @@
     </row>
     <row r="57" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
+      <c r="B57" s="20"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2870,7 +2868,7 @@
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
-      <c r="U57" s="20"/>
+      <c r="U57" s="1"/>
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
@@ -2878,7 +2876,7 @@
     </row>
     <row r="58" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
+      <c r="B58" s="20"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -2897,7 +2895,7 @@
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
-      <c r="U58" s="20"/>
+      <c r="U58" s="1"/>
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
@@ -2905,7 +2903,7 @@
     </row>
     <row r="59" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
+      <c r="B59" s="20"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -2924,7 +2922,7 @@
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
-      <c r="U59" s="20"/>
+      <c r="U59" s="1"/>
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
@@ -2932,7 +2930,7 @@
     </row>
     <row r="60" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
+      <c r="B60" s="20"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -2951,7 +2949,7 @@
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
-      <c r="U60" s="20"/>
+      <c r="U60" s="1"/>
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
@@ -2959,7 +2957,7 @@
     </row>
     <row r="61" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
+      <c r="B61" s="20"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -2978,7 +2976,7 @@
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
-      <c r="U61" s="20"/>
+      <c r="U61" s="1"/>
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
       <c r="X61" s="1"/>
@@ -2986,7 +2984,7 @@
     </row>
     <row r="62" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
+      <c r="B62" s="20"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -3005,7 +3003,7 @@
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
-      <c r="U62" s="20"/>
+      <c r="U62" s="1"/>
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
@@ -3013,7 +3011,7 @@
     </row>
     <row r="63" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
+      <c r="B63" s="20"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -3032,7 +3030,7 @@
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
-      <c r="U63" s="20"/>
+      <c r="U63" s="1"/>
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
       <c r="X63" s="1"/>
@@ -3040,7 +3038,7 @@
     </row>
     <row r="64" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
+      <c r="B64" s="20"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -3059,7 +3057,7 @@
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
-      <c r="U64" s="20"/>
+      <c r="U64" s="1"/>
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
@@ -3067,7 +3065,7 @@
     </row>
     <row r="65" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
+      <c r="B65" s="20"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -3086,7 +3084,7 @@
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
-      <c r="U65" s="20"/>
+      <c r="U65" s="1"/>
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
       <c r="X65" s="1"/>
@@ -3094,7 +3092,7 @@
     </row>
     <row r="66" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
+      <c r="B66" s="20"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -3113,7 +3111,7 @@
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
-      <c r="U66" s="20"/>
+      <c r="U66" s="1"/>
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
@@ -3121,7 +3119,7 @@
     </row>
     <row r="67" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
+      <c r="B67" s="20"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -3140,7 +3138,7 @@
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
-      <c r="U67" s="20"/>
+      <c r="U67" s="1"/>
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
       <c r="X67" s="1"/>
@@ -3148,7 +3146,7 @@
     </row>
     <row r="68" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
+      <c r="B68" s="20"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -3167,7 +3165,7 @@
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
-      <c r="U68" s="20"/>
+      <c r="U68" s="1"/>
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
       <c r="X68" s="1"/>
@@ -3175,7 +3173,7 @@
     </row>
     <row r="69" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
+      <c r="B69" s="20"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -3194,7 +3192,7 @@
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
-      <c r="U69" s="20"/>
+      <c r="U69" s="1"/>
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
       <c r="X69" s="1"/>
@@ -3202,7 +3200,7 @@
     </row>
     <row r="70" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
+      <c r="B70" s="20"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -3221,7 +3219,7 @@
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
-      <c r="U70" s="20"/>
+      <c r="U70" s="1"/>
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
       <c r="X70" s="1"/>
@@ -3229,7 +3227,7 @@
     </row>
     <row r="71" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
+      <c r="B71" s="20"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -3248,7 +3246,7 @@
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
-      <c r="U71" s="20"/>
+      <c r="U71" s="1"/>
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
       <c r="X71" s="1"/>
@@ -3256,7 +3254,7 @@
     </row>
     <row r="72" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
+      <c r="B72" s="20"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -3275,7 +3273,7 @@
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
-      <c r="U72" s="20"/>
+      <c r="U72" s="1"/>
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
       <c r="X72" s="1"/>
@@ -3283,7 +3281,7 @@
     </row>
     <row r="73" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+      <c r="B73" s="20"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -3302,7 +3300,7 @@
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
-      <c r="U73" s="20"/>
+      <c r="U73" s="1"/>
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
       <c r="X73" s="1"/>
@@ -3310,7 +3308,7 @@
     </row>
     <row r="74" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
+      <c r="B74" s="20"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -3329,7 +3327,7 @@
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
-      <c r="U74" s="20"/>
+      <c r="U74" s="1"/>
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
       <c r="X74" s="1"/>
@@ -3337,7 +3335,7 @@
     </row>
     <row r="75" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
+      <c r="B75" s="20"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -3356,7 +3354,7 @@
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
-      <c r="U75" s="20"/>
+      <c r="U75" s="1"/>
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
       <c r="X75" s="1"/>
@@ -3364,7 +3362,7 @@
     </row>
     <row r="76" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
+      <c r="B76" s="20"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -3383,7 +3381,7 @@
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
-      <c r="U76" s="20"/>
+      <c r="U76" s="1"/>
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
       <c r="X76" s="1"/>
@@ -3391,7 +3389,7 @@
     </row>
     <row r="77" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
+      <c r="B77" s="20"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -3410,7 +3408,7 @@
       <c r="R77" s="1"/>
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
-      <c r="U77" s="20"/>
+      <c r="U77" s="1"/>
       <c r="V77" s="1"/>
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
@@ -3418,7 +3416,7 @@
     </row>
     <row r="78" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
+      <c r="B78" s="20"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -3437,7 +3435,7 @@
       <c r="R78" s="1"/>
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
-      <c r="U78" s="20"/>
+      <c r="U78" s="1"/>
       <c r="V78" s="1"/>
       <c r="W78" s="1"/>
       <c r="X78" s="1"/>
@@ -3445,7 +3443,7 @@
     </row>
     <row r="79" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
+      <c r="B79" s="20"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -3464,7 +3462,7 @@
       <c r="R79" s="1"/>
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
-      <c r="U79" s="20"/>
+      <c r="U79" s="1"/>
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
@@ -3472,7 +3470,7 @@
     </row>
     <row r="80" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
+      <c r="B80" s="20"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -3491,7 +3489,7 @@
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
       <c r="T80" s="1"/>
-      <c r="U80" s="20"/>
+      <c r="U80" s="1"/>
       <c r="V80" s="1"/>
       <c r="W80" s="1"/>
       <c r="X80" s="1"/>
@@ -3499,7 +3497,7 @@
     </row>
     <row r="81" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
+      <c r="B81" s="20"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -3518,7 +3516,7 @@
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
-      <c r="U81" s="20"/>
+      <c r="U81" s="1"/>
       <c r="V81" s="1"/>
       <c r="W81" s="1"/>
       <c r="X81" s="1"/>
@@ -3526,7 +3524,7 @@
     </row>
     <row r="82" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
+      <c r="B82" s="20"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -3545,7 +3543,7 @@
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
-      <c r="U82" s="20"/>
+      <c r="U82" s="1"/>
       <c r="V82" s="1"/>
       <c r="W82" s="1"/>
       <c r="X82" s="1"/>
@@ -3553,7 +3551,7 @@
     </row>
     <row r="83" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
+      <c r="B83" s="20"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -3572,7 +3570,7 @@
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
-      <c r="U83" s="20"/>
+      <c r="U83" s="1"/>
       <c r="V83" s="1"/>
       <c r="W83" s="1"/>
       <c r="X83" s="1"/>
@@ -3580,7 +3578,7 @@
     </row>
     <row r="84" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
+      <c r="B84" s="20"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -3599,7 +3597,7 @@
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
       <c r="T84" s="1"/>
-      <c r="U84" s="20"/>
+      <c r="U84" s="1"/>
       <c r="V84" s="1"/>
       <c r="W84" s="1"/>
       <c r="X84" s="1"/>
@@ -3607,7 +3605,7 @@
     </row>
     <row r="85" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
+      <c r="B85" s="20"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -3626,7 +3624,7 @@
       <c r="R85" s="1"/>
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
-      <c r="U85" s="20"/>
+      <c r="U85" s="1"/>
       <c r="V85" s="1"/>
       <c r="W85" s="1"/>
       <c r="X85" s="1"/>
@@ -3634,7 +3632,7 @@
     </row>
     <row r="86" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
+      <c r="B86" s="20"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -3653,7 +3651,7 @@
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
       <c r="T86" s="1"/>
-      <c r="U86" s="20"/>
+      <c r="U86" s="1"/>
       <c r="V86" s="1"/>
       <c r="W86" s="1"/>
       <c r="X86" s="1"/>
@@ -3661,7 +3659,7 @@
     </row>
     <row r="87" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
+      <c r="B87" s="20"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -3680,7 +3678,7 @@
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
-      <c r="U87" s="20"/>
+      <c r="U87" s="1"/>
       <c r="V87" s="1"/>
       <c r="W87" s="1"/>
       <c r="X87" s="1"/>
@@ -3688,7 +3686,7 @@
     </row>
     <row r="88" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
+      <c r="B88" s="20"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -3707,7 +3705,7 @@
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
       <c r="T88" s="1"/>
-      <c r="U88" s="20"/>
+      <c r="U88" s="1"/>
       <c r="V88" s="1"/>
       <c r="W88" s="1"/>
       <c r="X88" s="1"/>
@@ -3715,7 +3713,7 @@
     </row>
     <row r="89" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
+      <c r="B89" s="20"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -3734,7 +3732,7 @@
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
-      <c r="U89" s="20"/>
+      <c r="U89" s="1"/>
       <c r="V89" s="1"/>
       <c r="W89" s="1"/>
       <c r="X89" s="1"/>
@@ -3742,7 +3740,7 @@
     </row>
     <row r="90" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
+      <c r="B90" s="20"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -3761,7 +3759,7 @@
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
       <c r="T90" s="1"/>
-      <c r="U90" s="20"/>
+      <c r="U90" s="1"/>
       <c r="V90" s="1"/>
       <c r="W90" s="1"/>
       <c r="X90" s="1"/>
@@ -3769,7 +3767,7 @@
     </row>
     <row r="91" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
+      <c r="B91" s="20"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -3788,7 +3786,7 @@
       <c r="R91" s="1"/>
       <c r="S91" s="1"/>
       <c r="T91" s="1"/>
-      <c r="U91" s="20"/>
+      <c r="U91" s="1"/>
       <c r="V91" s="1"/>
       <c r="W91" s="1"/>
       <c r="X91" s="1"/>
@@ -3796,7 +3794,7 @@
     </row>
     <row r="92" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
+      <c r="B92" s="20"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -3815,7 +3813,7 @@
       <c r="R92" s="1"/>
       <c r="S92" s="1"/>
       <c r="T92" s="1"/>
-      <c r="U92" s="20"/>
+      <c r="U92" s="1"/>
       <c r="V92" s="1"/>
       <c r="W92" s="1"/>
       <c r="X92" s="1"/>
@@ -3823,7 +3821,7 @@
     </row>
     <row r="93" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
+      <c r="B93" s="20"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -3842,7 +3840,7 @@
       <c r="R93" s="1"/>
       <c r="S93" s="1"/>
       <c r="T93" s="1"/>
-      <c r="U93" s="20"/>
+      <c r="U93" s="1"/>
       <c r="V93" s="1"/>
       <c r="W93" s="1"/>
       <c r="X93" s="1"/>
@@ -3850,7 +3848,7 @@
     </row>
     <row r="94" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
+      <c r="B94" s="20"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -3869,7 +3867,7 @@
       <c r="R94" s="1"/>
       <c r="S94" s="1"/>
       <c r="T94" s="1"/>
-      <c r="U94" s="20"/>
+      <c r="U94" s="1"/>
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
       <c r="X94" s="1"/>
@@ -3877,7 +3875,7 @@
     </row>
     <row r="95" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
+      <c r="B95" s="20"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -3896,7 +3894,7 @@
       <c r="R95" s="1"/>
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
-      <c r="U95" s="20"/>
+      <c r="U95" s="1"/>
       <c r="V95" s="1"/>
       <c r="W95" s="1"/>
       <c r="X95" s="1"/>
@@ -3904,7 +3902,7 @@
     </row>
     <row r="96" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
+      <c r="B96" s="20"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -3923,7 +3921,7 @@
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
       <c r="T96" s="1"/>
-      <c r="U96" s="20"/>
+      <c r="U96" s="1"/>
       <c r="V96" s="1"/>
       <c r="W96" s="1"/>
       <c r="X96" s="1"/>
@@ -3931,7 +3929,7 @@
     </row>
     <row r="97" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
+      <c r="B97" s="20"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -3950,7 +3948,7 @@
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
       <c r="T97" s="1"/>
-      <c r="U97" s="20"/>
+      <c r="U97" s="1"/>
       <c r="V97" s="1"/>
       <c r="W97" s="1"/>
       <c r="X97" s="1"/>
@@ -3958,7 +3956,7 @@
     </row>
     <row r="98" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
+      <c r="B98" s="20"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -3977,7 +3975,7 @@
       <c r="R98" s="1"/>
       <c r="S98" s="1"/>
       <c r="T98" s="1"/>
-      <c r="U98" s="20"/>
+      <c r="U98" s="1"/>
       <c r="V98" s="1"/>
       <c r="W98" s="1"/>
       <c r="X98" s="1"/>
@@ -3985,7 +3983,7 @@
     </row>
     <row r="99" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
+      <c r="B99" s="20"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -4004,7 +4002,7 @@
       <c r="R99" s="1"/>
       <c r="S99" s="1"/>
       <c r="T99" s="1"/>
-      <c r="U99" s="20"/>
+      <c r="U99" s="1"/>
       <c r="V99" s="1"/>
       <c r="W99" s="1"/>
       <c r="X99" s="1"/>
@@ -4012,7 +4010,7 @@
     </row>
     <row r="100" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
+      <c r="B100" s="20"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -4031,7 +4029,7 @@
       <c r="R100" s="1"/>
       <c r="S100" s="1"/>
       <c r="T100" s="1"/>
-      <c r="U100" s="20"/>
+      <c r="U100" s="1"/>
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
       <c r="X100" s="1"/>
@@ -4039,7 +4037,7 @@
     </row>
     <row r="101" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
+      <c r="B101" s="20"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -4058,7 +4056,7 @@
       <c r="R101" s="1"/>
       <c r="S101" s="1"/>
       <c r="T101" s="1"/>
-      <c r="U101" s="20"/>
+      <c r="U101" s="1"/>
       <c r="V101" s="1"/>
       <c r="W101" s="1"/>
       <c r="X101" s="1"/>
@@ -4066,7 +4064,7 @@
     </row>
     <row r="102" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
+      <c r="B102" s="20"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -4085,7 +4083,7 @@
       <c r="R102" s="1"/>
       <c r="S102" s="1"/>
       <c r="T102" s="1"/>
-      <c r="U102" s="20"/>
+      <c r="U102" s="1"/>
       <c r="V102" s="1"/>
       <c r="W102" s="1"/>
       <c r="X102" s="1"/>
@@ -4093,7 +4091,7 @@
     </row>
     <row r="103" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
+      <c r="B103" s="20"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -4112,7 +4110,7 @@
       <c r="R103" s="1"/>
       <c r="S103" s="1"/>
       <c r="T103" s="1"/>
-      <c r="U103" s="20"/>
+      <c r="U103" s="1"/>
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
       <c r="X103" s="1"/>
@@ -4120,7 +4118,7 @@
     </row>
     <row r="104" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
+      <c r="B104" s="20"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -4139,7 +4137,7 @@
       <c r="R104" s="1"/>
       <c r="S104" s="1"/>
       <c r="T104" s="1"/>
-      <c r="U104" s="20"/>
+      <c r="U104" s="1"/>
       <c r="V104" s="1"/>
       <c r="W104" s="1"/>
       <c r="X104" s="1"/>
@@ -4147,7 +4145,7 @@
     </row>
     <row r="105" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
+      <c r="B105" s="20"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -4166,7 +4164,7 @@
       <c r="R105" s="1"/>
       <c r="S105" s="1"/>
       <c r="T105" s="1"/>
-      <c r="U105" s="20"/>
+      <c r="U105" s="1"/>
       <c r="V105" s="1"/>
       <c r="W105" s="1"/>
       <c r="X105" s="1"/>
@@ -4174,7 +4172,7 @@
     </row>
     <row r="106" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
+      <c r="B106" s="20"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
@@ -4193,7 +4191,7 @@
       <c r="R106" s="1"/>
       <c r="S106" s="1"/>
       <c r="T106" s="1"/>
-      <c r="U106" s="20"/>
+      <c r="U106" s="1"/>
       <c r="V106" s="1"/>
       <c r="W106" s="1"/>
       <c r="X106" s="1"/>
@@ -4201,7 +4199,7 @@
     </row>
     <row r="107" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
+      <c r="B107" s="20"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
@@ -4220,7 +4218,7 @@
       <c r="R107" s="1"/>
       <c r="S107" s="1"/>
       <c r="T107" s="1"/>
-      <c r="U107" s="20"/>
+      <c r="U107" s="1"/>
       <c r="V107" s="1"/>
       <c r="W107" s="1"/>
       <c r="X107" s="1"/>
@@ -4228,7 +4226,7 @@
     </row>
     <row r="108" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
+      <c r="B108" s="20"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
@@ -4247,7 +4245,7 @@
       <c r="R108" s="1"/>
       <c r="S108" s="1"/>
       <c r="T108" s="1"/>
-      <c r="U108" s="20"/>
+      <c r="U108" s="1"/>
       <c r="V108" s="1"/>
       <c r="W108" s="1"/>
       <c r="X108" s="1"/>
@@ -4255,7 +4253,7 @@
     </row>
     <row r="109" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
+      <c r="B109" s="20"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -4274,7 +4272,7 @@
       <c r="R109" s="1"/>
       <c r="S109" s="1"/>
       <c r="T109" s="1"/>
-      <c r="U109" s="20"/>
+      <c r="U109" s="1"/>
       <c r="V109" s="1"/>
       <c r="W109" s="1"/>
       <c r="X109" s="1"/>
@@ -4282,7 +4280,7 @@
     </row>
     <row r="110" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
+      <c r="B110" s="20"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -4301,7 +4299,7 @@
       <c r="R110" s="1"/>
       <c r="S110" s="1"/>
       <c r="T110" s="1"/>
-      <c r="U110" s="20"/>
+      <c r="U110" s="1"/>
       <c r="V110" s="1"/>
       <c r="W110" s="1"/>
       <c r="X110" s="1"/>
@@ -4309,7 +4307,7 @@
     </row>
     <row r="111" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
+      <c r="B111" s="20"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -4328,7 +4326,7 @@
       <c r="R111" s="1"/>
       <c r="S111" s="1"/>
       <c r="T111" s="1"/>
-      <c r="U111" s="20"/>
+      <c r="U111" s="1"/>
       <c r="V111" s="1"/>
       <c r="W111" s="1"/>
       <c r="X111" s="1"/>
@@ -4336,7 +4334,7 @@
     </row>
     <row r="112" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
+      <c r="B112" s="20"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
@@ -4355,7 +4353,7 @@
       <c r="R112" s="1"/>
       <c r="S112" s="1"/>
       <c r="T112" s="1"/>
-      <c r="U112" s="20"/>
+      <c r="U112" s="1"/>
       <c r="V112" s="1"/>
       <c r="W112" s="1"/>
       <c r="X112" s="1"/>
@@ -4363,7 +4361,7 @@
     </row>
     <row r="113" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
+      <c r="B113" s="20"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -4382,7 +4380,7 @@
       <c r="R113" s="1"/>
       <c r="S113" s="1"/>
       <c r="T113" s="1"/>
-      <c r="U113" s="20"/>
+      <c r="U113" s="1"/>
       <c r="V113" s="1"/>
       <c r="W113" s="1"/>
       <c r="X113" s="1"/>
@@ -4390,7 +4388,7 @@
     </row>
     <row r="114" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
+      <c r="B114" s="20"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -4409,7 +4407,7 @@
       <c r="R114" s="1"/>
       <c r="S114" s="1"/>
       <c r="T114" s="1"/>
-      <c r="U114" s="20"/>
+      <c r="U114" s="1"/>
       <c r="V114" s="1"/>
       <c r="W114" s="1"/>
       <c r="X114" s="1"/>
@@ -4417,7 +4415,7 @@
     </row>
     <row r="115" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
+      <c r="B115" s="20"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -4436,7 +4434,7 @@
       <c r="R115" s="1"/>
       <c r="S115" s="1"/>
       <c r="T115" s="1"/>
-      <c r="U115" s="20"/>
+      <c r="U115" s="1"/>
       <c r="V115" s="1"/>
       <c r="W115" s="1"/>
       <c r="X115" s="1"/>
@@ -4444,7 +4442,7 @@
     </row>
     <row r="116" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
+      <c r="B116" s="20"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -4463,7 +4461,7 @@
       <c r="R116" s="1"/>
       <c r="S116" s="1"/>
       <c r="T116" s="1"/>
-      <c r="U116" s="20"/>
+      <c r="U116" s="1"/>
       <c r="V116" s="1"/>
       <c r="W116" s="1"/>
       <c r="X116" s="1"/>
@@ -4471,7 +4469,7 @@
     </row>
     <row r="117" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
+      <c r="B117" s="20"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -4490,7 +4488,7 @@
       <c r="R117" s="1"/>
       <c r="S117" s="1"/>
       <c r="T117" s="1"/>
-      <c r="U117" s="20"/>
+      <c r="U117" s="1"/>
       <c r="V117" s="1"/>
       <c r="W117" s="1"/>
       <c r="X117" s="1"/>
@@ -4498,7 +4496,7 @@
     </row>
     <row r="118" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
+      <c r="B118" s="20"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -4517,7 +4515,7 @@
       <c r="R118" s="1"/>
       <c r="S118" s="1"/>
       <c r="T118" s="1"/>
-      <c r="U118" s="20"/>
+      <c r="U118" s="1"/>
       <c r="V118" s="1"/>
       <c r="W118" s="1"/>
       <c r="X118" s="1"/>
@@ -4525,7 +4523,7 @@
     </row>
     <row r="119" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
+      <c r="B119" s="20"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -4544,7 +4542,7 @@
       <c r="R119" s="1"/>
       <c r="S119" s="1"/>
       <c r="T119" s="1"/>
-      <c r="U119" s="20"/>
+      <c r="U119" s="1"/>
       <c r="V119" s="1"/>
       <c r="W119" s="1"/>
       <c r="X119" s="1"/>
@@ -4552,7 +4550,7 @@
     </row>
     <row r="120" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
+      <c r="B120" s="20"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -4571,7 +4569,7 @@
       <c r="R120" s="1"/>
       <c r="S120" s="1"/>
       <c r="T120" s="1"/>
-      <c r="U120" s="20"/>
+      <c r="U120" s="1"/>
       <c r="V120" s="1"/>
       <c r="W120" s="1"/>
       <c r="X120" s="1"/>
@@ -4579,7 +4577,7 @@
     </row>
     <row r="121" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
+      <c r="B121" s="20"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -4598,7 +4596,7 @@
       <c r="R121" s="1"/>
       <c r="S121" s="1"/>
       <c r="T121" s="1"/>
-      <c r="U121" s="20"/>
+      <c r="U121" s="1"/>
       <c r="V121" s="1"/>
       <c r="W121" s="1"/>
       <c r="X121" s="1"/>
@@ -4606,7 +4604,7 @@
     </row>
     <row r="122" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
+      <c r="B122" s="20"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -4625,7 +4623,7 @@
       <c r="R122" s="1"/>
       <c r="S122" s="1"/>
       <c r="T122" s="1"/>
-      <c r="U122" s="20"/>
+      <c r="U122" s="1"/>
       <c r="V122" s="1"/>
       <c r="W122" s="1"/>
       <c r="X122" s="1"/>
@@ -4633,7 +4631,7 @@
     </row>
     <row r="123" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
+      <c r="B123" s="20"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -4652,7 +4650,7 @@
       <c r="R123" s="1"/>
       <c r="S123" s="1"/>
       <c r="T123" s="1"/>
-      <c r="U123" s="20"/>
+      <c r="U123" s="1"/>
       <c r="V123" s="1"/>
       <c r="W123" s="1"/>
       <c r="X123" s="1"/>
@@ -4660,7 +4658,7 @@
     </row>
     <row r="124" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
+      <c r="B124" s="20"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
@@ -4679,7 +4677,7 @@
       <c r="R124" s="1"/>
       <c r="S124" s="1"/>
       <c r="T124" s="1"/>
-      <c r="U124" s="20"/>
+      <c r="U124" s="1"/>
       <c r="V124" s="1"/>
       <c r="W124" s="1"/>
       <c r="X124" s="1"/>
@@ -4687,7 +4685,7 @@
     </row>
     <row r="125" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
+      <c r="B125" s="20"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -4706,7 +4704,7 @@
       <c r="R125" s="1"/>
       <c r="S125" s="1"/>
       <c r="T125" s="1"/>
-      <c r="U125" s="20"/>
+      <c r="U125" s="1"/>
       <c r="V125" s="1"/>
       <c r="W125" s="1"/>
       <c r="X125" s="1"/>
@@ -4714,7 +4712,7 @@
     </row>
     <row r="126" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
+      <c r="B126" s="20"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
@@ -4733,7 +4731,7 @@
       <c r="R126" s="1"/>
       <c r="S126" s="1"/>
       <c r="T126" s="1"/>
-      <c r="U126" s="20"/>
+      <c r="U126" s="1"/>
       <c r="V126" s="1"/>
       <c r="W126" s="1"/>
       <c r="X126" s="1"/>
@@ -4741,7 +4739,7 @@
     </row>
     <row r="127" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
+      <c r="B127" s="20"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -4760,7 +4758,7 @@
       <c r="R127" s="1"/>
       <c r="S127" s="1"/>
       <c r="T127" s="1"/>
-      <c r="U127" s="20"/>
+      <c r="U127" s="1"/>
       <c r="V127" s="1"/>
       <c r="W127" s="1"/>
       <c r="X127" s="1"/>
@@ -4768,7 +4766,7 @@
     </row>
     <row r="128" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
+      <c r="B128" s="20"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -4787,7 +4785,7 @@
       <c r="R128" s="1"/>
       <c r="S128" s="1"/>
       <c r="T128" s="1"/>
-      <c r="U128" s="20"/>
+      <c r="U128" s="1"/>
       <c r="V128" s="1"/>
       <c r="W128" s="1"/>
       <c r="X128" s="1"/>
@@ -4795,7 +4793,7 @@
     </row>
     <row r="129" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
+      <c r="B129" s="20"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -4814,7 +4812,7 @@
       <c r="R129" s="1"/>
       <c r="S129" s="1"/>
       <c r="T129" s="1"/>
-      <c r="U129" s="20"/>
+      <c r="U129" s="1"/>
       <c r="V129" s="1"/>
       <c r="W129" s="1"/>
       <c r="X129" s="1"/>
@@ -4822,7 +4820,7 @@
     </row>
     <row r="130" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
+      <c r="B130" s="20"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -4841,7 +4839,7 @@
       <c r="R130" s="1"/>
       <c r="S130" s="1"/>
       <c r="T130" s="1"/>
-      <c r="U130" s="20"/>
+      <c r="U130" s="1"/>
       <c r="V130" s="1"/>
       <c r="W130" s="1"/>
       <c r="X130" s="1"/>
@@ -4849,7 +4847,7 @@
     </row>
     <row r="131" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
-      <c r="B131" s="1"/>
+      <c r="B131" s="20"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -4868,7 +4866,7 @@
       <c r="R131" s="1"/>
       <c r="S131" s="1"/>
       <c r="T131" s="1"/>
-      <c r="U131" s="20"/>
+      <c r="U131" s="1"/>
       <c r="V131" s="1"/>
       <c r="W131" s="1"/>
       <c r="X131" s="1"/>
@@ -4876,7 +4874,7 @@
     </row>
     <row r="132" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
+      <c r="B132" s="20"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -4895,7 +4893,7 @@
       <c r="R132" s="1"/>
       <c r="S132" s="1"/>
       <c r="T132" s="1"/>
-      <c r="U132" s="20"/>
+      <c r="U132" s="1"/>
       <c r="V132" s="1"/>
       <c r="W132" s="1"/>
       <c r="X132" s="1"/>
@@ -4903,7 +4901,7 @@
     </row>
     <row r="133" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
-      <c r="B133" s="1"/>
+      <c r="B133" s="20"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
@@ -4922,7 +4920,7 @@
       <c r="R133" s="1"/>
       <c r="S133" s="1"/>
       <c r="T133" s="1"/>
-      <c r="U133" s="20"/>
+      <c r="U133" s="1"/>
       <c r="V133" s="1"/>
       <c r="W133" s="1"/>
       <c r="X133" s="1"/>
@@ -4930,7 +4928,7 @@
     </row>
     <row r="134" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
+      <c r="B134" s="20"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -4949,7 +4947,7 @@
       <c r="R134" s="1"/>
       <c r="S134" s="1"/>
       <c r="T134" s="1"/>
-      <c r="U134" s="20"/>
+      <c r="U134" s="1"/>
       <c r="V134" s="1"/>
       <c r="W134" s="1"/>
       <c r="X134" s="1"/>
@@ -4957,7 +4955,7 @@
     </row>
     <row r="135" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
-      <c r="B135" s="1"/>
+      <c r="B135" s="20"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -4976,7 +4974,7 @@
       <c r="R135" s="1"/>
       <c r="S135" s="1"/>
       <c r="T135" s="1"/>
-      <c r="U135" s="20"/>
+      <c r="U135" s="1"/>
       <c r="V135" s="1"/>
       <c r="W135" s="1"/>
       <c r="X135" s="1"/>
@@ -4984,7 +4982,7 @@
     </row>
     <row r="136" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
-      <c r="B136" s="1"/>
+      <c r="B136" s="20"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
@@ -5003,7 +5001,7 @@
       <c r="R136" s="1"/>
       <c r="S136" s="1"/>
       <c r="T136" s="1"/>
-      <c r="U136" s="20"/>
+      <c r="U136" s="1"/>
       <c r="V136" s="1"/>
       <c r="W136" s="1"/>
       <c r="X136" s="1"/>
@@ -5011,7 +5009,7 @@
     </row>
     <row r="137" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
-      <c r="B137" s="1"/>
+      <c r="B137" s="20"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -5030,7 +5028,7 @@
       <c r="R137" s="1"/>
       <c r="S137" s="1"/>
       <c r="T137" s="1"/>
-      <c r="U137" s="20"/>
+      <c r="U137" s="1"/>
       <c r="V137" s="1"/>
       <c r="W137" s="1"/>
       <c r="X137" s="1"/>
@@ -5038,7 +5036,7 @@
     </row>
     <row r="138" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
+      <c r="B138" s="20"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
@@ -5057,7 +5055,7 @@
       <c r="R138" s="1"/>
       <c r="S138" s="1"/>
       <c r="T138" s="1"/>
-      <c r="U138" s="20"/>
+      <c r="U138" s="1"/>
       <c r="V138" s="1"/>
       <c r="W138" s="1"/>
       <c r="X138" s="1"/>
@@ -5065,7 +5063,7 @@
     </row>
     <row r="139" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
-      <c r="B139" s="1"/>
+      <c r="B139" s="20"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -5084,7 +5082,7 @@
       <c r="R139" s="1"/>
       <c r="S139" s="1"/>
       <c r="T139" s="1"/>
-      <c r="U139" s="20"/>
+      <c r="U139" s="1"/>
       <c r="V139" s="1"/>
       <c r="W139" s="1"/>
       <c r="X139" s="1"/>
@@ -5092,7 +5090,7 @@
     </row>
     <row r="140" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
-      <c r="B140" s="1"/>
+      <c r="B140" s="20"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
@@ -5111,7 +5109,7 @@
       <c r="R140" s="1"/>
       <c r="S140" s="1"/>
       <c r="T140" s="1"/>
-      <c r="U140" s="20"/>
+      <c r="U140" s="1"/>
       <c r="V140" s="1"/>
       <c r="W140" s="1"/>
       <c r="X140" s="1"/>
@@ -5119,7 +5117,7 @@
     </row>
     <row r="141" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
-      <c r="B141" s="1"/>
+      <c r="B141" s="20"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
@@ -5138,7 +5136,7 @@
       <c r="R141" s="1"/>
       <c r="S141" s="1"/>
       <c r="T141" s="1"/>
-      <c r="U141" s="20"/>
+      <c r="U141" s="1"/>
       <c r="V141" s="1"/>
       <c r="W141" s="1"/>
       <c r="X141" s="1"/>
@@ -5146,7 +5144,7 @@
     </row>
     <row r="142" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
-      <c r="B142" s="1"/>
+      <c r="B142" s="20"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -5165,7 +5163,7 @@
       <c r="R142" s="1"/>
       <c r="S142" s="1"/>
       <c r="T142" s="1"/>
-      <c r="U142" s="20"/>
+      <c r="U142" s="1"/>
       <c r="V142" s="1"/>
       <c r="W142" s="1"/>
       <c r="X142" s="1"/>
@@ -5173,7 +5171,7 @@
     </row>
     <row r="143" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
-      <c r="B143" s="1"/>
+      <c r="B143" s="20"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
@@ -5192,7 +5190,7 @@
       <c r="R143" s="1"/>
       <c r="S143" s="1"/>
       <c r="T143" s="1"/>
-      <c r="U143" s="20"/>
+      <c r="U143" s="1"/>
       <c r="V143" s="1"/>
       <c r="W143" s="1"/>
       <c r="X143" s="1"/>
@@ -5200,7 +5198,7 @@
     </row>
     <row r="144" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
+      <c r="B144" s="20"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
@@ -5219,7 +5217,7 @@
       <c r="R144" s="1"/>
       <c r="S144" s="1"/>
       <c r="T144" s="1"/>
-      <c r="U144" s="20"/>
+      <c r="U144" s="1"/>
       <c r="V144" s="1"/>
       <c r="W144" s="1"/>
       <c r="X144" s="1"/>
@@ -5227,7 +5225,7 @@
     </row>
     <row r="145" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
-      <c r="B145" s="1"/>
+      <c r="B145" s="20"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -5246,7 +5244,7 @@
       <c r="R145" s="1"/>
       <c r="S145" s="1"/>
       <c r="T145" s="1"/>
-      <c r="U145" s="20"/>
+      <c r="U145" s="1"/>
       <c r="V145" s="1"/>
       <c r="W145" s="1"/>
       <c r="X145" s="1"/>
@@ -5254,7 +5252,7 @@
     </row>
     <row r="146" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
-      <c r="B146" s="1"/>
+      <c r="B146" s="20"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -5273,7 +5271,7 @@
       <c r="R146" s="1"/>
       <c r="S146" s="1"/>
       <c r="T146" s="1"/>
-      <c r="U146" s="20"/>
+      <c r="U146" s="1"/>
       <c r="V146" s="1"/>
       <c r="W146" s="1"/>
       <c r="X146" s="1"/>
@@ -5281,7 +5279,7 @@
     </row>
     <row r="147" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
+      <c r="B147" s="20"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -5300,7 +5298,7 @@
       <c r="R147" s="1"/>
       <c r="S147" s="1"/>
       <c r="T147" s="1"/>
-      <c r="U147" s="20"/>
+      <c r="U147" s="1"/>
       <c r="V147" s="1"/>
       <c r="W147" s="1"/>
       <c r="X147" s="1"/>
@@ -5308,7 +5306,7 @@
     </row>
     <row r="148" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
-      <c r="B148" s="1"/>
+      <c r="B148" s="20"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -5327,7 +5325,7 @@
       <c r="R148" s="1"/>
       <c r="S148" s="1"/>
       <c r="T148" s="1"/>
-      <c r="U148" s="20"/>
+      <c r="U148" s="1"/>
       <c r="V148" s="1"/>
       <c r="W148" s="1"/>
       <c r="X148" s="1"/>
@@ -5335,7 +5333,7 @@
     </row>
     <row r="149" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
-      <c r="B149" s="1"/>
+      <c r="B149" s="20"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -5354,7 +5352,7 @@
       <c r="R149" s="1"/>
       <c r="S149" s="1"/>
       <c r="T149" s="1"/>
-      <c r="U149" s="20"/>
+      <c r="U149" s="1"/>
       <c r="V149" s="1"/>
       <c r="W149" s="1"/>
       <c r="X149" s="1"/>
@@ -5362,7 +5360,7 @@
     </row>
     <row r="150" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
+      <c r="B150" s="20"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -5381,7 +5379,7 @@
       <c r="R150" s="1"/>
       <c r="S150" s="1"/>
       <c r="T150" s="1"/>
-      <c r="U150" s="20"/>
+      <c r="U150" s="1"/>
       <c r="V150" s="1"/>
       <c r="W150" s="1"/>
       <c r="X150" s="1"/>
@@ -5389,7 +5387,7 @@
     </row>
     <row r="151" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
-      <c r="B151" s="1"/>
+      <c r="B151" s="20"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -5408,7 +5406,7 @@
       <c r="R151" s="1"/>
       <c r="S151" s="1"/>
       <c r="T151" s="1"/>
-      <c r="U151" s="20"/>
+      <c r="U151" s="1"/>
       <c r="V151" s="1"/>
       <c r="W151" s="1"/>
       <c r="X151" s="1"/>
@@ -5416,7 +5414,7 @@
     </row>
     <row r="152" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
+      <c r="B152" s="20"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -5435,7 +5433,7 @@
       <c r="R152" s="1"/>
       <c r="S152" s="1"/>
       <c r="T152" s="1"/>
-      <c r="U152" s="20"/>
+      <c r="U152" s="1"/>
       <c r="V152" s="1"/>
       <c r="W152" s="1"/>
       <c r="X152" s="1"/>
@@ -5443,7 +5441,7 @@
     </row>
     <row r="153" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
+      <c r="B153" s="20"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
@@ -5462,7 +5460,7 @@
       <c r="R153" s="1"/>
       <c r="S153" s="1"/>
       <c r="T153" s="1"/>
-      <c r="U153" s="20"/>
+      <c r="U153" s="1"/>
       <c r="V153" s="1"/>
       <c r="W153" s="1"/>
       <c r="X153" s="1"/>
@@ -5470,7 +5468,7 @@
     </row>
     <row r="154" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
-      <c r="B154" s="1"/>
+      <c r="B154" s="20"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -5489,7 +5487,7 @@
       <c r="R154" s="1"/>
       <c r="S154" s="1"/>
       <c r="T154" s="1"/>
-      <c r="U154" s="20"/>
+      <c r="U154" s="1"/>
       <c r="V154" s="1"/>
       <c r="W154" s="1"/>
       <c r="X154" s="1"/>
@@ -5497,7 +5495,7 @@
     </row>
     <row r="155" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
-      <c r="B155" s="1"/>
+      <c r="B155" s="20"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -5516,7 +5514,7 @@
       <c r="R155" s="1"/>
       <c r="S155" s="1"/>
       <c r="T155" s="1"/>
-      <c r="U155" s="20"/>
+      <c r="U155" s="1"/>
       <c r="V155" s="1"/>
       <c r="W155" s="1"/>
       <c r="X155" s="1"/>
@@ -5524,7 +5522,7 @@
     </row>
     <row r="156" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
+      <c r="B156" s="20"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
@@ -5543,7 +5541,7 @@
       <c r="R156" s="1"/>
       <c r="S156" s="1"/>
       <c r="T156" s="1"/>
-      <c r="U156" s="20"/>
+      <c r="U156" s="1"/>
       <c r="V156" s="1"/>
       <c r="W156" s="1"/>
       <c r="X156" s="1"/>
@@ -5551,7 +5549,7 @@
     </row>
     <row r="157" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
-      <c r="B157" s="1"/>
+      <c r="B157" s="20"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
       <c r="E157" s="1"/>
@@ -5570,7 +5568,7 @@
       <c r="R157" s="1"/>
       <c r="S157" s="1"/>
       <c r="T157" s="1"/>
-      <c r="U157" s="20"/>
+      <c r="U157" s="1"/>
       <c r="V157" s="1"/>
       <c r="W157" s="1"/>
       <c r="X157" s="1"/>
@@ -5578,7 +5576,7 @@
     </row>
     <row r="158" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
+      <c r="B158" s="20"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
       <c r="E158" s="1"/>
@@ -5597,7 +5595,7 @@
       <c r="R158" s="1"/>
       <c r="S158" s="1"/>
       <c r="T158" s="1"/>
-      <c r="U158" s="20"/>
+      <c r="U158" s="1"/>
       <c r="V158" s="1"/>
       <c r="W158" s="1"/>
       <c r="X158" s="1"/>
@@ -5605,7 +5603,7 @@
     </row>
     <row r="159" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
+      <c r="B159" s="20"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
@@ -5624,7 +5622,7 @@
       <c r="R159" s="1"/>
       <c r="S159" s="1"/>
       <c r="T159" s="1"/>
-      <c r="U159" s="20"/>
+      <c r="U159" s="1"/>
       <c r="V159" s="1"/>
       <c r="W159" s="1"/>
       <c r="X159" s="1"/>
@@ -5632,7 +5630,7 @@
     </row>
     <row r="160" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
-      <c r="B160" s="1"/>
+      <c r="B160" s="20"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
@@ -5651,7 +5649,7 @@
       <c r="R160" s="1"/>
       <c r="S160" s="1"/>
       <c r="T160" s="1"/>
-      <c r="U160" s="20"/>
+      <c r="U160" s="1"/>
       <c r="V160" s="1"/>
       <c r="W160" s="1"/>
       <c r="X160" s="1"/>
@@ -5659,7 +5657,7 @@
     </row>
     <row r="161" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
-      <c r="B161" s="1"/>
+      <c r="B161" s="20"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
@@ -5678,7 +5676,7 @@
       <c r="R161" s="1"/>
       <c r="S161" s="1"/>
       <c r="T161" s="1"/>
-      <c r="U161" s="20"/>
+      <c r="U161" s="1"/>
       <c r="V161" s="1"/>
       <c r="W161" s="1"/>
       <c r="X161" s="1"/>
@@ -5686,7 +5684,7 @@
     </row>
     <row r="162" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
+      <c r="B162" s="20"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
@@ -5705,7 +5703,7 @@
       <c r="R162" s="1"/>
       <c r="S162" s="1"/>
       <c r="T162" s="1"/>
-      <c r="U162" s="20"/>
+      <c r="U162" s="1"/>
       <c r="V162" s="1"/>
       <c r="W162" s="1"/>
       <c r="X162" s="1"/>
@@ -5713,7 +5711,7 @@
     </row>
     <row r="163" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
-      <c r="B163" s="1"/>
+      <c r="B163" s="20"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
@@ -5732,7 +5730,7 @@
       <c r="R163" s="1"/>
       <c r="S163" s="1"/>
       <c r="T163" s="1"/>
-      <c r="U163" s="20"/>
+      <c r="U163" s="1"/>
       <c r="V163" s="1"/>
       <c r="W163" s="1"/>
       <c r="X163" s="1"/>
@@ -5740,7 +5738,7 @@
     </row>
     <row r="164" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
-      <c r="B164" s="1"/>
+      <c r="B164" s="20"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
@@ -5759,7 +5757,7 @@
       <c r="R164" s="1"/>
       <c r="S164" s="1"/>
       <c r="T164" s="1"/>
-      <c r="U164" s="20"/>
+      <c r="U164" s="1"/>
       <c r="V164" s="1"/>
       <c r="W164" s="1"/>
       <c r="X164" s="1"/>
@@ -5767,7 +5765,7 @@
     </row>
     <row r="165" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
+      <c r="B165" s="20"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
@@ -5786,7 +5784,7 @@
       <c r="R165" s="1"/>
       <c r="S165" s="1"/>
       <c r="T165" s="1"/>
-      <c r="U165" s="20"/>
+      <c r="U165" s="1"/>
       <c r="V165" s="1"/>
       <c r="W165" s="1"/>
       <c r="X165" s="1"/>
@@ -5794,7 +5792,7 @@
     </row>
     <row r="166" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
+      <c r="B166" s="20"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
@@ -5813,7 +5811,7 @@
       <c r="R166" s="1"/>
       <c r="S166" s="1"/>
       <c r="T166" s="1"/>
-      <c r="U166" s="20"/>
+      <c r="U166" s="1"/>
       <c r="V166" s="1"/>
       <c r="W166" s="1"/>
       <c r="X166" s="1"/>
@@ -5821,7 +5819,7 @@
     </row>
     <row r="167" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
-      <c r="B167" s="1"/>
+      <c r="B167" s="20"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
@@ -5840,7 +5838,7 @@
       <c r="R167" s="1"/>
       <c r="S167" s="1"/>
       <c r="T167" s="1"/>
-      <c r="U167" s="20"/>
+      <c r="U167" s="1"/>
       <c r="V167" s="1"/>
       <c r="W167" s="1"/>
       <c r="X167" s="1"/>
@@ -5848,7 +5846,7 @@
     </row>
     <row r="168" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
-      <c r="B168" s="1"/>
+      <c r="B168" s="20"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
       <c r="E168" s="1"/>
@@ -5867,7 +5865,7 @@
       <c r="R168" s="1"/>
       <c r="S168" s="1"/>
       <c r="T168" s="1"/>
-      <c r="U168" s="20"/>
+      <c r="U168" s="1"/>
       <c r="V168" s="1"/>
       <c r="W168" s="1"/>
       <c r="X168" s="1"/>
@@ -5875,7 +5873,7 @@
     </row>
     <row r="169" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
-      <c r="B169" s="1"/>
+      <c r="B169" s="20"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
@@ -5894,7 +5892,7 @@
       <c r="R169" s="1"/>
       <c r="S169" s="1"/>
       <c r="T169" s="1"/>
-      <c r="U169" s="20"/>
+      <c r="U169" s="1"/>
       <c r="V169" s="1"/>
       <c r="W169" s="1"/>
       <c r="X169" s="1"/>
@@ -5902,7 +5900,7 @@
     </row>
     <row r="170" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
-      <c r="B170" s="1"/>
+      <c r="B170" s="20"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
@@ -5921,7 +5919,7 @@
       <c r="R170" s="1"/>
       <c r="S170" s="1"/>
       <c r="T170" s="1"/>
-      <c r="U170" s="20"/>
+      <c r="U170" s="1"/>
       <c r="V170" s="1"/>
       <c r="W170" s="1"/>
       <c r="X170" s="1"/>
@@ -5929,7 +5927,7 @@
     </row>
     <row r="171" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
+      <c r="B171" s="20"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
@@ -5948,7 +5946,7 @@
       <c r="R171" s="1"/>
       <c r="S171" s="1"/>
       <c r="T171" s="1"/>
-      <c r="U171" s="20"/>
+      <c r="U171" s="1"/>
       <c r="V171" s="1"/>
       <c r="W171" s="1"/>
       <c r="X171" s="1"/>
@@ -5956,7 +5954,7 @@
     </row>
     <row r="172" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
-      <c r="B172" s="1"/>
+      <c r="B172" s="20"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
@@ -5975,7 +5973,7 @@
       <c r="R172" s="1"/>
       <c r="S172" s="1"/>
       <c r="T172" s="1"/>
-      <c r="U172" s="20"/>
+      <c r="U172" s="1"/>
       <c r="V172" s="1"/>
       <c r="W172" s="1"/>
       <c r="X172" s="1"/>
@@ -5983,7 +5981,7 @@
     </row>
     <row r="173" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
-      <c r="B173" s="1"/>
+      <c r="B173" s="20"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -6002,7 +6000,7 @@
       <c r="R173" s="1"/>
       <c r="S173" s="1"/>
       <c r="T173" s="1"/>
-      <c r="U173" s="20"/>
+      <c r="U173" s="1"/>
       <c r="V173" s="1"/>
       <c r="W173" s="1"/>
       <c r="X173" s="1"/>
@@ -6010,7 +6008,7 @@
     </row>
     <row r="174" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
-      <c r="B174" s="1"/>
+      <c r="B174" s="20"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
@@ -6029,7 +6027,7 @@
       <c r="R174" s="1"/>
       <c r="S174" s="1"/>
       <c r="T174" s="1"/>
-      <c r="U174" s="20"/>
+      <c r="U174" s="1"/>
       <c r="V174" s="1"/>
       <c r="W174" s="1"/>
       <c r="X174" s="1"/>
@@ -6037,7 +6035,7 @@
     </row>
     <row r="175" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
-      <c r="B175" s="1"/>
+      <c r="B175" s="20"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -6056,7 +6054,7 @@
       <c r="R175" s="1"/>
       <c r="S175" s="1"/>
       <c r="T175" s="1"/>
-      <c r="U175" s="20"/>
+      <c r="U175" s="1"/>
       <c r="V175" s="1"/>
       <c r="W175" s="1"/>
       <c r="X175" s="1"/>
@@ -6064,7 +6062,7 @@
     </row>
     <row r="176" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
-      <c r="B176" s="1"/>
+      <c r="B176" s="20"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
@@ -6083,7 +6081,7 @@
       <c r="R176" s="1"/>
       <c r="S176" s="1"/>
       <c r="T176" s="1"/>
-      <c r="U176" s="20"/>
+      <c r="U176" s="1"/>
       <c r="V176" s="1"/>
       <c r="W176" s="1"/>
       <c r="X176" s="1"/>
@@ -6091,7 +6089,7 @@
     </row>
     <row r="177" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
+      <c r="B177" s="20"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
       <c r="E177" s="1"/>
@@ -6110,7 +6108,7 @@
       <c r="R177" s="1"/>
       <c r="S177" s="1"/>
       <c r="T177" s="1"/>
-      <c r="U177" s="20"/>
+      <c r="U177" s="1"/>
       <c r="V177" s="1"/>
       <c r="W177" s="1"/>
       <c r="X177" s="1"/>
@@ -6118,7 +6116,7 @@
     </row>
     <row r="178" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
-      <c r="B178" s="1"/>
+      <c r="B178" s="20"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
@@ -6137,7 +6135,7 @@
       <c r="R178" s="1"/>
       <c r="S178" s="1"/>
       <c r="T178" s="1"/>
-      <c r="U178" s="20"/>
+      <c r="U178" s="1"/>
       <c r="V178" s="1"/>
       <c r="W178" s="1"/>
       <c r="X178" s="1"/>
@@ -6145,7 +6143,7 @@
     </row>
     <row r="179" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
-      <c r="B179" s="1"/>
+      <c r="B179" s="20"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
@@ -6164,7 +6162,7 @@
       <c r="R179" s="1"/>
       <c r="S179" s="1"/>
       <c r="T179" s="1"/>
-      <c r="U179" s="20"/>
+      <c r="U179" s="1"/>
       <c r="V179" s="1"/>
       <c r="W179" s="1"/>
       <c r="X179" s="1"/>
@@ -6172,7 +6170,7 @@
     </row>
     <row r="180" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
-      <c r="B180" s="1"/>
+      <c r="B180" s="20"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
       <c r="E180" s="1"/>
@@ -6191,7 +6189,7 @@
       <c r="R180" s="1"/>
       <c r="S180" s="1"/>
       <c r="T180" s="1"/>
-      <c r="U180" s="20"/>
+      <c r="U180" s="1"/>
       <c r="V180" s="1"/>
       <c r="W180" s="1"/>
       <c r="X180" s="1"/>
@@ -6199,7 +6197,7 @@
     </row>
     <row r="181" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
-      <c r="B181" s="1"/>
+      <c r="B181" s="20"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
@@ -6218,7 +6216,7 @@
       <c r="R181" s="1"/>
       <c r="S181" s="1"/>
       <c r="T181" s="1"/>
-      <c r="U181" s="20"/>
+      <c r="U181" s="1"/>
       <c r="V181" s="1"/>
       <c r="W181" s="1"/>
       <c r="X181" s="1"/>
@@ -6226,7 +6224,7 @@
     </row>
     <row r="182" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
-      <c r="B182" s="1"/>
+      <c r="B182" s="20"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
@@ -6245,7 +6243,7 @@
       <c r="R182" s="1"/>
       <c r="S182" s="1"/>
       <c r="T182" s="1"/>
-      <c r="U182" s="20"/>
+      <c r="U182" s="1"/>
       <c r="V182" s="1"/>
       <c r="W182" s="1"/>
       <c r="X182" s="1"/>
@@ -6253,7 +6251,7 @@
     </row>
     <row r="183" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
-      <c r="B183" s="1"/>
+      <c r="B183" s="20"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
@@ -6272,7 +6270,7 @@
       <c r="R183" s="1"/>
       <c r="S183" s="1"/>
       <c r="T183" s="1"/>
-      <c r="U183" s="20"/>
+      <c r="U183" s="1"/>
       <c r="V183" s="1"/>
       <c r="W183" s="1"/>
       <c r="X183" s="1"/>
@@ -6280,7 +6278,7 @@
     </row>
     <row r="184" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
-      <c r="B184" s="1"/>
+      <c r="B184" s="20"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
@@ -6299,7 +6297,7 @@
       <c r="R184" s="1"/>
       <c r="S184" s="1"/>
       <c r="T184" s="1"/>
-      <c r="U184" s="20"/>
+      <c r="U184" s="1"/>
       <c r="V184" s="1"/>
       <c r="W184" s="1"/>
       <c r="X184" s="1"/>
@@ -6307,7 +6305,7 @@
     </row>
     <row r="185" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
-      <c r="B185" s="1"/>
+      <c r="B185" s="20"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
@@ -6326,7 +6324,7 @@
       <c r="R185" s="1"/>
       <c r="S185" s="1"/>
       <c r="T185" s="1"/>
-      <c r="U185" s="20"/>
+      <c r="U185" s="1"/>
       <c r="V185" s="1"/>
       <c r="W185" s="1"/>
       <c r="X185" s="1"/>
@@ -6334,7 +6332,7 @@
     </row>
     <row r="186" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
-      <c r="B186" s="1"/>
+      <c r="B186" s="20"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
@@ -6353,7 +6351,7 @@
       <c r="R186" s="1"/>
       <c r="S186" s="1"/>
       <c r="T186" s="1"/>
-      <c r="U186" s="20"/>
+      <c r="U186" s="1"/>
       <c r="V186" s="1"/>
       <c r="W186" s="1"/>
       <c r="X186" s="1"/>
@@ -6361,7 +6359,7 @@
     </row>
     <row r="187" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
-      <c r="B187" s="1"/>
+      <c r="B187" s="20"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
@@ -6380,7 +6378,7 @@
       <c r="R187" s="1"/>
       <c r="S187" s="1"/>
       <c r="T187" s="1"/>
-      <c r="U187" s="20"/>
+      <c r="U187" s="1"/>
       <c r="V187" s="1"/>
       <c r="W187" s="1"/>
       <c r="X187" s="1"/>
@@ -6388,7 +6386,7 @@
     </row>
     <row r="188" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
-      <c r="B188" s="1"/>
+      <c r="B188" s="20"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
@@ -6407,7 +6405,7 @@
       <c r="R188" s="1"/>
       <c r="S188" s="1"/>
       <c r="T188" s="1"/>
-      <c r="U188" s="20"/>
+      <c r="U188" s="1"/>
       <c r="V188" s="1"/>
       <c r="W188" s="1"/>
       <c r="X188" s="1"/>
@@ -6415,7 +6413,7 @@
     </row>
     <row r="189" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
-      <c r="B189" s="1"/>
+      <c r="B189" s="20"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
@@ -6434,7 +6432,7 @@
       <c r="R189" s="1"/>
       <c r="S189" s="1"/>
       <c r="T189" s="1"/>
-      <c r="U189" s="20"/>
+      <c r="U189" s="1"/>
       <c r="V189" s="1"/>
       <c r="W189" s="1"/>
       <c r="X189" s="1"/>
@@ -6442,7 +6440,7 @@
     </row>
     <row r="190" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
-      <c r="B190" s="1"/>
+      <c r="B190" s="20"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
@@ -6461,7 +6459,7 @@
       <c r="R190" s="1"/>
       <c r="S190" s="1"/>
       <c r="T190" s="1"/>
-      <c r="U190" s="20"/>
+      <c r="U190" s="1"/>
       <c r="V190" s="1"/>
       <c r="W190" s="1"/>
       <c r="X190" s="1"/>
@@ -6469,7 +6467,7 @@
     </row>
     <row r="191" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
-      <c r="B191" s="1"/>
+      <c r="B191" s="20"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
@@ -6488,7 +6486,7 @@
       <c r="R191" s="1"/>
       <c r="S191" s="1"/>
       <c r="T191" s="1"/>
-      <c r="U191" s="20"/>
+      <c r="U191" s="1"/>
       <c r="V191" s="1"/>
       <c r="W191" s="1"/>
       <c r="X191" s="1"/>
@@ -6496,7 +6494,7 @@
     </row>
     <row r="192" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
-      <c r="B192" s="1"/>
+      <c r="B192" s="20"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
       <c r="E192" s="1"/>
@@ -6515,7 +6513,7 @@
       <c r="R192" s="1"/>
       <c r="S192" s="1"/>
       <c r="T192" s="1"/>
-      <c r="U192" s="20"/>
+      <c r="U192" s="1"/>
       <c r="V192" s="1"/>
       <c r="W192" s="1"/>
       <c r="X192" s="1"/>
@@ -6523,7 +6521,7 @@
     </row>
     <row r="193" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
-      <c r="B193" s="1"/>
+      <c r="B193" s="20"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
@@ -6542,7 +6540,7 @@
       <c r="R193" s="1"/>
       <c r="S193" s="1"/>
       <c r="T193" s="1"/>
-      <c r="U193" s="20"/>
+      <c r="U193" s="1"/>
       <c r="V193" s="1"/>
       <c r="W193" s="1"/>
       <c r="X193" s="1"/>
@@ -6550,7 +6548,7 @@
     </row>
     <row r="194" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
-      <c r="B194" s="1"/>
+      <c r="B194" s="20"/>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
@@ -6569,7 +6567,7 @@
       <c r="R194" s="1"/>
       <c r="S194" s="1"/>
       <c r="T194" s="1"/>
-      <c r="U194" s="20"/>
+      <c r="U194" s="1"/>
       <c r="V194" s="1"/>
       <c r="W194" s="1"/>
       <c r="X194" s="1"/>
@@ -6577,7 +6575,7 @@
     </row>
     <row r="195" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
-      <c r="B195" s="1"/>
+      <c r="B195" s="20"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
@@ -6596,7 +6594,7 @@
       <c r="R195" s="1"/>
       <c r="S195" s="1"/>
       <c r="T195" s="1"/>
-      <c r="U195" s="20"/>
+      <c r="U195" s="1"/>
       <c r="V195" s="1"/>
       <c r="W195" s="1"/>
       <c r="X195" s="1"/>
@@ -6604,7 +6602,7 @@
     </row>
     <row r="196" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
-      <c r="B196" s="1"/>
+      <c r="B196" s="20"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
@@ -6623,7 +6621,7 @@
       <c r="R196" s="1"/>
       <c r="S196" s="1"/>
       <c r="T196" s="1"/>
-      <c r="U196" s="20"/>
+      <c r="U196" s="1"/>
       <c r="V196" s="1"/>
       <c r="W196" s="1"/>
       <c r="X196" s="1"/>
@@ -6631,7 +6629,7 @@
     </row>
     <row r="197" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
-      <c r="B197" s="1"/>
+      <c r="B197" s="20"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
@@ -6650,7 +6648,7 @@
       <c r="R197" s="1"/>
       <c r="S197" s="1"/>
       <c r="T197" s="1"/>
-      <c r="U197" s="20"/>
+      <c r="U197" s="1"/>
       <c r="V197" s="1"/>
       <c r="W197" s="1"/>
       <c r="X197" s="1"/>
@@ -6658,7 +6656,7 @@
     </row>
     <row r="198" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
-      <c r="B198" s="1"/>
+      <c r="B198" s="20"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
@@ -6677,7 +6675,7 @@
       <c r="R198" s="1"/>
       <c r="S198" s="1"/>
       <c r="T198" s="1"/>
-      <c r="U198" s="20"/>
+      <c r="U198" s="1"/>
       <c r="V198" s="1"/>
       <c r="W198" s="1"/>
       <c r="X198" s="1"/>
@@ -6685,7 +6683,7 @@
     </row>
     <row r="199" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
-      <c r="B199" s="1"/>
+      <c r="B199" s="20"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
@@ -6704,7 +6702,7 @@
       <c r="R199" s="1"/>
       <c r="S199" s="1"/>
       <c r="T199" s="1"/>
-      <c r="U199" s="20"/>
+      <c r="U199" s="1"/>
       <c r="V199" s="1"/>
       <c r="W199" s="1"/>
       <c r="X199" s="1"/>
@@ -6712,7 +6710,7 @@
     </row>
     <row r="200" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
-      <c r="B200" s="1"/>
+      <c r="B200" s="20"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
@@ -6731,7 +6729,7 @@
       <c r="R200" s="1"/>
       <c r="S200" s="1"/>
       <c r="T200" s="1"/>
-      <c r="U200" s="20"/>
+      <c r="U200" s="1"/>
       <c r="V200" s="1"/>
       <c r="W200" s="1"/>
       <c r="X200" s="1"/>
@@ -6739,7 +6737,7 @@
     </row>
     <row r="201" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
-      <c r="B201" s="1"/>
+      <c r="B201" s="20"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
@@ -6758,7 +6756,7 @@
       <c r="R201" s="1"/>
       <c r="S201" s="1"/>
       <c r="T201" s="1"/>
-      <c r="U201" s="20"/>
+      <c r="U201" s="1"/>
       <c r="V201" s="1"/>
       <c r="W201" s="1"/>
       <c r="X201" s="1"/>
@@ -6766,7 +6764,7 @@
     </row>
     <row r="202" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
-      <c r="B202" s="1"/>
+      <c r="B202" s="20"/>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
@@ -6785,7 +6783,7 @@
       <c r="R202" s="1"/>
       <c r="S202" s="1"/>
       <c r="T202" s="1"/>
-      <c r="U202" s="20"/>
+      <c r="U202" s="1"/>
       <c r="V202" s="1"/>
       <c r="W202" s="1"/>
       <c r="X202" s="1"/>
@@ -6793,7 +6791,7 @@
     </row>
     <row r="203" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
-      <c r="B203" s="1"/>
+      <c r="B203" s="20"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
       <c r="E203" s="1"/>
@@ -6812,7 +6810,7 @@
       <c r="R203" s="1"/>
       <c r="S203" s="1"/>
       <c r="T203" s="1"/>
-      <c r="U203" s="20"/>
+      <c r="U203" s="1"/>
       <c r="V203" s="1"/>
       <c r="W203" s="1"/>
       <c r="X203" s="1"/>
@@ -6820,7 +6818,7 @@
     </row>
     <row r="204" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
-      <c r="B204" s="1"/>
+      <c r="B204" s="20"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
       <c r="E204" s="1"/>
@@ -6839,7 +6837,7 @@
       <c r="R204" s="1"/>
       <c r="S204" s="1"/>
       <c r="T204" s="1"/>
-      <c r="U204" s="20"/>
+      <c r="U204" s="1"/>
       <c r="V204" s="1"/>
       <c r="W204" s="1"/>
       <c r="X204" s="1"/>
@@ -6847,7 +6845,7 @@
     </row>
     <row r="205" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
-      <c r="B205" s="1"/>
+      <c r="B205" s="20"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
@@ -6866,7 +6864,7 @@
       <c r="R205" s="1"/>
       <c r="S205" s="1"/>
       <c r="T205" s="1"/>
-      <c r="U205" s="20"/>
+      <c r="U205" s="1"/>
       <c r="V205" s="1"/>
       <c r="W205" s="1"/>
       <c r="X205" s="1"/>
@@ -6874,7 +6872,7 @@
     </row>
     <row r="206" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
-      <c r="B206" s="1"/>
+      <c r="B206" s="20"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
@@ -6893,7 +6891,7 @@
       <c r="R206" s="1"/>
       <c r="S206" s="1"/>
       <c r="T206" s="1"/>
-      <c r="U206" s="20"/>
+      <c r="U206" s="1"/>
       <c r="V206" s="1"/>
       <c r="W206" s="1"/>
       <c r="X206" s="1"/>
@@ -6901,7 +6899,7 @@
     </row>
     <row r="207" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
-      <c r="B207" s="1"/>
+      <c r="B207" s="20"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
@@ -6920,7 +6918,7 @@
       <c r="R207" s="1"/>
       <c r="S207" s="1"/>
       <c r="T207" s="1"/>
-      <c r="U207" s="20"/>
+      <c r="U207" s="1"/>
       <c r="V207" s="1"/>
       <c r="W207" s="1"/>
       <c r="X207" s="1"/>
@@ -6928,7 +6926,7 @@
     </row>
     <row r="208" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
-      <c r="B208" s="1"/>
+      <c r="B208" s="20"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
@@ -6947,7 +6945,7 @@
       <c r="R208" s="1"/>
       <c r="S208" s="1"/>
       <c r="T208" s="1"/>
-      <c r="U208" s="20"/>
+      <c r="U208" s="1"/>
       <c r="V208" s="1"/>
       <c r="W208" s="1"/>
       <c r="X208" s="1"/>
@@ -6955,7 +6953,7 @@
     </row>
     <row r="209" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
-      <c r="B209" s="1"/>
+      <c r="B209" s="20"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
       <c r="E209" s="1"/>
@@ -6974,7 +6972,7 @@
       <c r="R209" s="1"/>
       <c r="S209" s="1"/>
       <c r="T209" s="1"/>
-      <c r="U209" s="20"/>
+      <c r="U209" s="1"/>
       <c r="V209" s="1"/>
       <c r="W209" s="1"/>
       <c r="X209" s="1"/>
@@ -6982,7 +6980,7 @@
     </row>
     <row r="210" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
-      <c r="B210" s="1"/>
+      <c r="B210" s="20"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
       <c r="E210" s="1"/>
@@ -7001,7 +6999,7 @@
       <c r="R210" s="1"/>
       <c r="S210" s="1"/>
       <c r="T210" s="1"/>
-      <c r="U210" s="20"/>
+      <c r="U210" s="1"/>
       <c r="V210" s="1"/>
       <c r="W210" s="1"/>
       <c r="X210" s="1"/>
@@ -7009,7 +7007,7 @@
     </row>
     <row r="211" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
-      <c r="B211" s="1"/>
+      <c r="B211" s="20"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
@@ -7028,7 +7026,7 @@
       <c r="R211" s="1"/>
       <c r="S211" s="1"/>
       <c r="T211" s="1"/>
-      <c r="U211" s="20"/>
+      <c r="U211" s="1"/>
       <c r="V211" s="1"/>
       <c r="W211" s="1"/>
       <c r="X211" s="1"/>
@@ -7036,7 +7034,7 @@
     </row>
     <row r="212" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
-      <c r="B212" s="1"/>
+      <c r="B212" s="20"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
       <c r="E212" s="1"/>
@@ -7055,7 +7053,7 @@
       <c r="R212" s="1"/>
       <c r="S212" s="1"/>
       <c r="T212" s="1"/>
-      <c r="U212" s="20"/>
+      <c r="U212" s="1"/>
       <c r="V212" s="1"/>
       <c r="W212" s="1"/>
       <c r="X212" s="1"/>
@@ -7063,7 +7061,7 @@
     </row>
     <row r="213" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
-      <c r="B213" s="1"/>
+      <c r="B213" s="20"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
       <c r="E213" s="1"/>
@@ -7082,7 +7080,7 @@
       <c r="R213" s="1"/>
       <c r="S213" s="1"/>
       <c r="T213" s="1"/>
-      <c r="U213" s="20"/>
+      <c r="U213" s="1"/>
       <c r="V213" s="1"/>
       <c r="W213" s="1"/>
       <c r="X213" s="1"/>
@@ -7090,7 +7088,7 @@
     </row>
     <row r="214" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
-      <c r="B214" s="1"/>
+      <c r="B214" s="20"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
       <c r="E214" s="1"/>
@@ -7109,7 +7107,7 @@
       <c r="R214" s="1"/>
       <c r="S214" s="1"/>
       <c r="T214" s="1"/>
-      <c r="U214" s="20"/>
+      <c r="U214" s="1"/>
       <c r="V214" s="1"/>
       <c r="W214" s="1"/>
       <c r="X214" s="1"/>
@@ -7117,7 +7115,7 @@
     </row>
     <row r="215" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
-      <c r="B215" s="1"/>
+      <c r="B215" s="20"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
@@ -7136,7 +7134,7 @@
       <c r="R215" s="1"/>
       <c r="S215" s="1"/>
       <c r="T215" s="1"/>
-      <c r="U215" s="20"/>
+      <c r="U215" s="1"/>
       <c r="V215" s="1"/>
       <c r="W215" s="1"/>
       <c r="X215" s="1"/>
@@ -7144,7 +7142,7 @@
     </row>
     <row r="216" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
-      <c r="B216" s="1"/>
+      <c r="B216" s="20"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
       <c r="E216" s="1"/>
@@ -7163,7 +7161,7 @@
       <c r="R216" s="1"/>
       <c r="S216" s="1"/>
       <c r="T216" s="1"/>
-      <c r="U216" s="20"/>
+      <c r="U216" s="1"/>
       <c r="V216" s="1"/>
       <c r="W216" s="1"/>
       <c r="X216" s="1"/>

</xml_diff>